<commit_message>
(67286, Gabriela Silva) Added sprint 6's second day management updates
</commit_message>
<xml_diff>
--- a/SE202526/Management/Sprint6/burndown/Sprint6_Burndown.xlsx
+++ b/SE202526/Management/Sprint6/burndown/Sprint6_Burndown.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\Sprint6\burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AEDA1E-BD0C-4EC8-BE8B-8CD079626636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A226766-D548-4920-BB42-22F70D7DD9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Sprint1" sheetId="1" r:id="rId1"/>
-    <sheet name="Folha2" sheetId="7" r:id="rId2"/>
-    <sheet name="Burndown Chart Sprint2" sheetId="2" r:id="rId3"/>
-    <sheet name="Burndown Chart Sprint3" sheetId="3" r:id="rId4"/>
-    <sheet name="Burndown Chart Sprint4" sheetId="4" r:id="rId5"/>
-    <sheet name="Burndown Chart Sprint5" sheetId="5" r:id="rId6"/>
-    <sheet name="Burndown Chart Sprint6" sheetId="6" r:id="rId7"/>
+    <sheet name="Burndown Chart Sprint2" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndown Chart Sprint3" sheetId="3" r:id="rId3"/>
+    <sheet name="Burndown Chart Sprint4" sheetId="4" r:id="rId4"/>
+    <sheet name="Burndown Chart Sprint5" sheetId="5" r:id="rId5"/>
+    <sheet name="Burndown Chart Sprint6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="118">
   <si>
     <t>Sprint 1 Burndown Chart</t>
   </si>
@@ -461,6 +460,24 @@
   <si>
     <t>Look into what a class diagram covering US2 would look like (liquid leak checking).</t>
   </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 4 Burndown Chart</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
 </sst>
 </file>
 
@@ -604,7 +621,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -1287,47 +1304,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -1369,17 +1345,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1393,17 +1402,6 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1414,7 +1412,52 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1422,7 +1465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1605,15 +1648,6 @@
     <xf numFmtId="164" fontId="3" fillId="9" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1623,43 +1657,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1671,16 +1675,38 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1733,7 +1759,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4625,10 +4651,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint6'!$D$38:$K$38</c:f>
+              <c:f>'Burndown Chart Sprint6'!$D$24:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4648,7 +4698,7 @@
               </c14:invertSolidFillFmt>
             </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A4D4-4742-81A4-441B273627E2}"/>
+              <c16:uniqueId val="{00000000-E343-48C0-ACE3-350B2A067F4F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4726,17 +4776,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint6'!$D$39:$K$39</c:f>
+              <c:f>'Burndown Chart Sprint6'!$D$25:$K$25</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A4D4-4742-81A4-441B273627E2}"/>
+              <c16:uniqueId val="{00000001-E343-48C0-ACE3-350B2A067F4F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4789,17 +4863,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint6'!$D$40:$K$40</c:f>
+              <c:f>'Burndown Chart Sprint6'!$D$26:$K$26</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8571428571428541</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.428571428571427</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A4D4-4742-81A4-441B273627E2}"/>
+              <c16:uniqueId val="{00000002-E343-48C0-ACE3-350B2A067F4F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4873,7 +4971,7 @@
         <c:axId val="1165773373"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16"/>
+          <c:max val="31"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5160,18 +5258,18 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1687286</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9639300" cy="4886325"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart">
+        <xdr:cNvPr id="4" name="Chart 3" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6275FD17-D533-4BF7-A893-F8C0FB6C9F43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE8AFAC6-399A-464C-B52A-C3C3883393EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5394,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5412,50 +5510,50 @@
   <sheetData>
     <row r="1" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="98"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="93"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="99" t="s">
+      <c r="E3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
       <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="98" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -5500,8 +5598,8 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="102"/>
-      <c r="C5" s="104"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="99"/>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
@@ -5722,10 +5820,10 @@
       <c r="P11" s="24"/>
     </row>
     <row r="12" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="106"/>
+      <c r="C12" s="101"/>
       <c r="D12" s="26">
         <v>0</v>
       </c>
@@ -5779,10 +5877,10 @@
       </c>
     </row>
     <row r="13" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="93"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="32">
         <f>SUM(D6:D12)</f>
         <v>14</v>
@@ -5837,10 +5935,10 @@
       </c>
     </row>
     <row r="14" spans="2:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="95"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="39">
         <f>D13</f>
         <v>14</v>
@@ -6897,23 +6995,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA02847-0711-498E-99DE-5C5B6511AE88}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6928,40 +7014,40 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="98"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="93"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
+      <c r="E3" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="98" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -6991,8 +7077,8 @@
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="102"/>
-      <c r="C5" s="104"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="99"/>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
@@ -7222,10 +7308,10 @@
       <c r="K14" s="22"/>
     </row>
     <row r="15" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="106"/>
+      <c r="C15" s="101"/>
       <c r="D15" s="26">
         <v>0</v>
       </c>
@@ -7259,10 +7345,10 @@
       </c>
     </row>
     <row r="16" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="93"/>
+      <c r="C16" s="88"/>
       <c r="D16" s="32">
         <f>SUM(D6:D15)</f>
         <v>6.5</v>
@@ -7297,10 +7383,10 @@
       </c>
     </row>
     <row r="17" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="95"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="39">
         <f>D16</f>
         <v>6.5</v>
@@ -8333,12 +8419,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8352,40 +8438,40 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
+      <c r="E3" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="98" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -8414,8 +8500,8 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="102"/>
-      <c r="C5" s="104"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="99"/>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
@@ -8460,11 +8546,11 @@
         <v>0.1</v>
       </c>
       <c r="K6" s="16"/>
-      <c r="L6" s="108" t="str">
+      <c r="L6" s="103" t="str">
         <f t="shared" ref="L6:L37" si="0">IF(N6=0, "NOT STARTED",IF(N6&gt;D6, "ERROR TO MUCH WORK", IF(N6=D6, "DONE", "NOT ENOUGH WORK YET")))</f>
         <v>DONE</v>
       </c>
-      <c r="M6" s="109"/>
+      <c r="M6" s="104"/>
       <c r="N6" s="44">
         <f t="shared" ref="N6:N37" si="1">SUM(E6:K6)</f>
         <v>0.1</v>
@@ -8495,11 +8581,11 @@
       <c r="I7" s="23"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
-      <c r="L7" s="108" t="str">
+      <c r="L7" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M7" s="109"/>
+      <c r="M7" s="104"/>
       <c r="N7" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -8534,11 +8620,11 @@
       <c r="K8" s="22">
         <v>0.15</v>
       </c>
-      <c r="L8" s="108" t="str">
+      <c r="L8" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M8" s="109"/>
+      <c r="M8" s="104"/>
       <c r="N8" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -8571,11 +8657,11 @@
         <v>0.25</v>
       </c>
       <c r="K9" s="22"/>
-      <c r="L9" s="108" t="str">
+      <c r="L9" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M9" s="109"/>
+      <c r="M9" s="104"/>
       <c r="N9" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -8608,11 +8694,11 @@
         <v>0.25</v>
       </c>
       <c r="K10" s="22"/>
-      <c r="L10" s="108" t="str">
+      <c r="L10" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M10" s="109"/>
+      <c r="M10" s="104"/>
       <c r="N10" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -8645,11 +8731,11 @@
       <c r="K11" s="22">
         <v>0.25</v>
       </c>
-      <c r="L11" s="108" t="str">
+      <c r="L11" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M11" s="109"/>
+      <c r="M11" s="104"/>
       <c r="N11" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -8680,11 +8766,11 @@
         <v>0.25</v>
       </c>
       <c r="K12" s="22"/>
-      <c r="L12" s="108" t="str">
+      <c r="L12" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M12" s="109"/>
+      <c r="M12" s="104"/>
       <c r="N12" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -8717,11 +8803,11 @@
       <c r="I13" s="23"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
-      <c r="L13" s="108" t="str">
+      <c r="L13" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M13" s="109"/>
+      <c r="M13" s="104"/>
       <c r="N13" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -8752,11 +8838,11 @@
       <c r="K14" s="22">
         <v>0.2</v>
       </c>
-      <c r="L14" s="108" t="str">
+      <c r="L14" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M14" s="109"/>
+      <c r="M14" s="104"/>
       <c r="N14" s="44">
         <f t="shared" si="1"/>
         <v>0.2</v>
@@ -8789,11 +8875,11 @@
       <c r="K15" s="22">
         <v>0.2</v>
       </c>
-      <c r="L15" s="108" t="str">
+      <c r="L15" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M15" s="109"/>
+      <c r="M15" s="104"/>
       <c r="N15" s="44">
         <f t="shared" si="1"/>
         <v>0.45</v>
@@ -8826,11 +8912,11 @@
         <v>0.3</v>
       </c>
       <c r="K16" s="22"/>
-      <c r="L16" s="108" t="str">
+      <c r="L16" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M16" s="109"/>
+      <c r="M16" s="104"/>
       <c r="N16" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -8863,11 +8949,11 @@
       <c r="K17" s="22">
         <v>0.2</v>
       </c>
-      <c r="L17" s="108" t="str">
+      <c r="L17" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M17" s="109"/>
+      <c r="M17" s="104"/>
       <c r="N17" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -8896,11 +8982,11 @@
       <c r="I18" s="23"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
-      <c r="L18" s="108" t="str">
+      <c r="L18" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M18" s="109"/>
+      <c r="M18" s="104"/>
       <c r="N18" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8933,11 +9019,11 @@
       </c>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
-      <c r="L19" s="108" t="str">
+      <c r="L19" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M19" s="109"/>
+      <c r="M19" s="104"/>
       <c r="N19" s="44">
         <f t="shared" si="1"/>
         <v>0.35</v>
@@ -8974,11 +9060,11 @@
       <c r="K20" s="22">
         <v>0.2</v>
       </c>
-      <c r="L20" s="108" t="str">
+      <c r="L20" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M20" s="109"/>
+      <c r="M20" s="104"/>
       <c r="N20" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -9013,11 +9099,11 @@
       <c r="K21" s="22">
         <v>0.2</v>
       </c>
-      <c r="L21" s="108" t="str">
+      <c r="L21" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M21" s="109"/>
+      <c r="M21" s="104"/>
       <c r="N21" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -9054,11 +9140,11 @@
       <c r="K22" s="22">
         <v>0.2</v>
       </c>
-      <c r="L22" s="108" t="str">
+      <c r="L22" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M22" s="109"/>
+      <c r="M22" s="104"/>
       <c r="N22" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -9089,11 +9175,11 @@
       <c r="K23" s="22">
         <v>0.25</v>
       </c>
-      <c r="L23" s="108" t="str">
+      <c r="L23" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M23" s="109"/>
+      <c r="M23" s="104"/>
       <c r="N23" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -9122,11 +9208,11 @@
       <c r="I24" s="23"/>
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
-      <c r="L24" s="108" t="str">
+      <c r="L24" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M24" s="109"/>
+      <c r="M24" s="104"/>
       <c r="N24" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9157,11 +9243,11 @@
       <c r="I25" s="23"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
-      <c r="L25" s="108" t="str">
+      <c r="L25" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M25" s="109"/>
+      <c r="M25" s="104"/>
       <c r="N25" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -9194,11 +9280,11 @@
         <v>0.25</v>
       </c>
       <c r="K26" s="22"/>
-      <c r="L26" s="108" t="str">
+      <c r="L26" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M26" s="109"/>
+      <c r="M26" s="104"/>
       <c r="N26" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -9233,11 +9319,11 @@
       <c r="K27" s="22">
         <v>0.1</v>
       </c>
-      <c r="L27" s="108" t="str">
+      <c r="L27" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M27" s="109"/>
+      <c r="M27" s="104"/>
       <c r="N27" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -9272,11 +9358,11 @@
       <c r="K28" s="22">
         <v>0.1</v>
       </c>
-      <c r="L28" s="108" t="str">
+      <c r="L28" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M28" s="109"/>
+      <c r="M28" s="104"/>
       <c r="N28" s="44">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -9307,11 +9393,11 @@
       <c r="K29" s="22">
         <v>0.2</v>
       </c>
-      <c r="L29" s="108" t="str">
+      <c r="L29" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M29" s="109"/>
+      <c r="M29" s="104"/>
       <c r="N29" s="44">
         <f t="shared" si="1"/>
         <v>0.2</v>
@@ -9340,11 +9426,11 @@
       <c r="I30" s="23"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
-      <c r="L30" s="108" t="str">
+      <c r="L30" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M30" s="109"/>
+      <c r="M30" s="104"/>
       <c r="N30" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9375,11 +9461,11 @@
       <c r="I31" s="23"/>
       <c r="J31" s="22"/>
       <c r="K31" s="22"/>
-      <c r="L31" s="108" t="str">
+      <c r="L31" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M31" s="109"/>
+      <c r="M31" s="104"/>
       <c r="N31" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -9412,11 +9498,11 @@
       <c r="K32" s="22">
         <v>0.15</v>
       </c>
-      <c r="L32" s="108" t="str">
+      <c r="L32" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M32" s="109"/>
+      <c r="M32" s="104"/>
       <c r="N32" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -9449,11 +9535,11 @@
       <c r="K33" s="49">
         <v>0.15</v>
       </c>
-      <c r="L33" s="108" t="str">
+      <c r="L33" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M33" s="109"/>
+      <c r="M33" s="104"/>
       <c r="N33" s="44">
         <f t="shared" si="1"/>
         <v>0.3</v>
@@ -9484,11 +9570,11 @@
       <c r="K34" s="49">
         <v>0.4</v>
       </c>
-      <c r="L34" s="108" t="str">
+      <c r="L34" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M34" s="109"/>
+      <c r="M34" s="104"/>
       <c r="N34" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -9517,11 +9603,11 @@
       <c r="I35" s="50"/>
       <c r="J35" s="51"/>
       <c r="K35" s="49"/>
-      <c r="L35" s="108" t="str">
+      <c r="L35" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M35" s="109"/>
+      <c r="M35" s="104"/>
       <c r="N35" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9550,11 +9636,11 @@
       <c r="I36" s="50"/>
       <c r="J36" s="51"/>
       <c r="K36" s="49"/>
-      <c r="L36" s="108" t="str">
+      <c r="L36" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M36" s="109"/>
+      <c r="M36" s="104"/>
       <c r="N36" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9585,11 +9671,11 @@
       </c>
       <c r="J37" s="51"/>
       <c r="K37" s="49"/>
-      <c r="L37" s="108" t="str">
+      <c r="L37" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M37" s="109"/>
+      <c r="M37" s="104"/>
       <c r="N37" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -9602,10 +9688,10 @@
       </c>
     </row>
     <row r="38" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="105" t="s">
+      <c r="B38" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="106"/>
+      <c r="C38" s="101"/>
       <c r="D38" s="26">
         <v>0</v>
       </c>
@@ -9639,10 +9725,10 @@
       </c>
     </row>
     <row r="39" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="93"/>
+      <c r="C39" s="88"/>
       <c r="D39" s="32">
         <f>SUM(D6:D38)</f>
         <v>15.6</v>
@@ -9676,11 +9762,11 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="40" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="94" t="s">
+    <row r="40" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="95"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="39">
         <v>15.6</v>
       </c>
@@ -10749,12 +10835,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P988"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10768,40 +10854,40 @@
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="107" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="B2" s="102" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
+      <c r="E3" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="98" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -10830,8 +10916,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="102"/>
-      <c r="C5" s="104"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="99"/>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
@@ -10879,11 +10965,11 @@
       <c r="I6" s="23"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
-      <c r="L6" s="108" t="str">
+      <c r="L6" s="103" t="str">
         <f t="shared" ref="L6:L25" si="0">IF(N6=0, "NOT STARTED",IF(N6&gt;D6, "ERROR TO MUCH WORK", IF(N6=D6, "DONE", "NOT ENOUGH WORK YET")))</f>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M6" s="109"/>
+      <c r="M6" s="104"/>
       <c r="N6" s="44">
         <f t="shared" ref="N6:N25" si="1">SUM(E6:K6)</f>
         <v>0.25</v>
@@ -10914,11 +11000,11 @@
         <v>0.25</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="L7" s="108" t="str">
+      <c r="L7" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M7" s="109"/>
+      <c r="M7" s="104"/>
       <c r="N7" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -10949,11 +11035,11 @@
       <c r="K8" s="22">
         <v>0.2</v>
       </c>
-      <c r="L8" s="108" t="str">
+      <c r="L8" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M8" s="109"/>
+      <c r="M8" s="104"/>
       <c r="N8" s="44">
         <f t="shared" si="1"/>
         <v>0.2</v>
@@ -10986,11 +11072,11 @@
       <c r="K9" s="22">
         <v>0.2</v>
       </c>
-      <c r="L9" s="108" t="str">
+      <c r="L9" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M9" s="109"/>
+      <c r="M9" s="104"/>
       <c r="N9" s="44">
         <f t="shared" si="1"/>
         <v>0.45</v>
@@ -11023,11 +11109,11 @@
         <v>0.3</v>
       </c>
       <c r="K10" s="22"/>
-      <c r="L10" s="108" t="str">
+      <c r="L10" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M10" s="109"/>
+      <c r="M10" s="104"/>
       <c r="N10" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -11060,11 +11146,11 @@
       <c r="K11" s="22">
         <v>0.2</v>
       </c>
-      <c r="L11" s="108" t="str">
+      <c r="L11" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M11" s="109"/>
+      <c r="M11" s="104"/>
       <c r="N11" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -11093,11 +11179,11 @@
       <c r="I12" s="23"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
-      <c r="L12" s="108" t="str">
+      <c r="L12" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M12" s="109"/>
+      <c r="M12" s="104"/>
       <c r="N12" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -11130,11 +11216,11 @@
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
-      <c r="L13" s="108" t="str">
+      <c r="L13" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M13" s="109"/>
+      <c r="M13" s="104"/>
       <c r="N13" s="44">
         <f t="shared" si="1"/>
         <v>0.35</v>
@@ -11165,11 +11251,11 @@
       <c r="K14" s="22">
         <v>0.25</v>
       </c>
-      <c r="L14" s="108" t="str">
+      <c r="L14" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M14" s="109"/>
+      <c r="M14" s="104"/>
       <c r="N14" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -11198,11 +11284,11 @@
       <c r="I15" s="23"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
-      <c r="L15" s="108" t="str">
+      <c r="L15" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M15" s="109"/>
+      <c r="M15" s="104"/>
       <c r="N15" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -11233,11 +11319,11 @@
       <c r="I16" s="23"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
-      <c r="L16" s="108" t="str">
+      <c r="L16" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M16" s="109"/>
+      <c r="M16" s="104"/>
       <c r="N16" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -11268,11 +11354,11 @@
       <c r="K17" s="22">
         <v>0.2</v>
       </c>
-      <c r="L17" s="108" t="str">
+      <c r="L17" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M17" s="109"/>
+      <c r="M17" s="104"/>
       <c r="N17" s="44">
         <f t="shared" si="1"/>
         <v>0.2</v>
@@ -11301,11 +11387,11 @@
       <c r="I18" s="23"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
-      <c r="L18" s="108" t="str">
+      <c r="L18" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M18" s="109"/>
+      <c r="M18" s="104"/>
       <c r="N18" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -11336,11 +11422,11 @@
       <c r="I19" s="23"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
-      <c r="L19" s="108" t="str">
+      <c r="L19" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M19" s="109"/>
+      <c r="M19" s="104"/>
       <c r="N19" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -11373,11 +11459,11 @@
       <c r="K20" s="22">
         <v>0.15</v>
       </c>
-      <c r="L20" s="108" t="str">
+      <c r="L20" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M20" s="109"/>
+      <c r="M20" s="104"/>
       <c r="N20" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -11410,11 +11496,11 @@
       <c r="K21" s="49">
         <v>0.15</v>
       </c>
-      <c r="L21" s="108" t="str">
+      <c r="L21" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M21" s="109"/>
+      <c r="M21" s="104"/>
       <c r="N21" s="44">
         <f t="shared" si="1"/>
         <v>0.3</v>
@@ -11445,11 +11531,11 @@
       <c r="K22" s="49">
         <v>0.4</v>
       </c>
-      <c r="L22" s="108" t="str">
+      <c r="L22" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M22" s="109"/>
+      <c r="M22" s="104"/>
       <c r="N22" s="44">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -11478,11 +11564,11 @@
       <c r="I23" s="50"/>
       <c r="J23" s="51"/>
       <c r="K23" s="49"/>
-      <c r="L23" s="108" t="str">
+      <c r="L23" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M23" s="109"/>
+      <c r="M23" s="104"/>
       <c r="N23" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -11511,11 +11597,11 @@
       <c r="I24" s="50"/>
       <c r="J24" s="51"/>
       <c r="K24" s="49"/>
-      <c r="L24" s="108" t="str">
+      <c r="L24" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M24" s="109"/>
+      <c r="M24" s="104"/>
       <c r="N24" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -11546,11 +11632,11 @@
       </c>
       <c r="J25" s="51"/>
       <c r="K25" s="49"/>
-      <c r="L25" s="108" t="str">
+      <c r="L25" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M25" s="109"/>
+      <c r="M25" s="104"/>
       <c r="N25" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -11563,10 +11649,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="105" t="s">
+      <c r="B26" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="106"/>
+      <c r="C26" s="101"/>
       <c r="D26" s="26">
         <v>0</v>
       </c>
@@ -11600,10 +11686,10 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="93"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="32">
         <f>SUM(D6:D26)</f>
         <v>10</v>
@@ -11638,10 +11724,10 @@
       </c>
     </row>
     <row r="28" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="95"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="39">
         <v>15.6</v>
       </c>
@@ -12698,12 +12784,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF431CF1-8E16-45D5-A381-7331DD95E65F}">
   <dimension ref="B1:P976"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12717,40 +12803,40 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
+      <c r="E3" s="94" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="98" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -12779,8 +12865,8 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="102"/>
-      <c r="C5" s="104"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="99"/>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
@@ -12831,11 +12917,11 @@
         <v>0.5</v>
       </c>
       <c r="K6" s="22"/>
-      <c r="L6" s="108" t="str">
+      <c r="L6" s="103" t="str">
         <f t="shared" ref="L6:L10" si="0">IF(N6=0, "NOT STARTED",IF(N6&gt;D6, "ERROR TO MUCH WORK", IF(N6=D6, "DONE", "NOT ENOUGH WORK YET")))</f>
         <v>DONE</v>
       </c>
-      <c r="M6" s="109"/>
+      <c r="M6" s="104"/>
       <c r="N6" s="44">
         <f t="shared" ref="N6:N10" si="1">SUM(E6:K6)</f>
         <v>2</v>
@@ -12868,11 +12954,11 @@
         <v>0.5</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="L7" s="108" t="str">
+      <c r="L7" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M7" s="109"/>
+      <c r="M7" s="104"/>
       <c r="N7" s="44">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -12907,11 +12993,11 @@
         <v>0.1</v>
       </c>
       <c r="K8" s="22"/>
-      <c r="L8" s="108" t="str">
+      <c r="L8" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M8" s="109"/>
+      <c r="M8" s="104"/>
       <c r="N8" s="44">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -12938,11 +13024,11 @@
       <c r="I9" s="23"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
-      <c r="L9" s="108" t="str">
+      <c r="L9" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M9" s="109"/>
+      <c r="M9" s="104"/>
       <c r="N9" s="44">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -12973,11 +13059,11 @@
       <c r="I10" s="23"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
-      <c r="L10" s="108" t="str">
+      <c r="L10" s="103" t="str">
         <f t="shared" si="0"/>
         <v>DONE</v>
       </c>
-      <c r="M10" s="109"/>
+      <c r="M10" s="104"/>
       <c r="N10" s="44">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -13012,11 +13098,11 @@
         <v>0.1</v>
       </c>
       <c r="K11" s="22"/>
-      <c r="L11" s="110" t="str">
+      <c r="L11" s="105" t="str">
         <f>IF(N11=0, "NOT STARTED",IF(N11&gt;D11, "ERROR TO MUCH WORK", IF(N11=D11, "DONE", "NOT ENOUGH WORK YET")))</f>
         <v>DONE</v>
       </c>
-      <c r="M11" s="111"/>
+      <c r="M11" s="106"/>
       <c r="N11" s="44">
         <f>SUM(E11:K11)</f>
         <v>2</v>
@@ -13045,11 +13131,11 @@
       <c r="K12" s="22">
         <v>0.6</v>
       </c>
-      <c r="L12" s="108" t="str">
+      <c r="L12" s="103" t="str">
         <f t="shared" ref="L12" si="2">IF(N12=0, "NOT STARTED",IF(N12&gt;D12, "ERROR TO MUCH WORK", IF(N12=D12, "DONE", "NOT ENOUGH WORK YET")))</f>
         <v>DONE</v>
       </c>
-      <c r="M12" s="109"/>
+      <c r="M12" s="104"/>
       <c r="N12" s="44">
         <f t="shared" ref="N12" si="3">SUM(E12:K12)</f>
         <v>1.6</v>
@@ -13076,11 +13162,11 @@
         <v>1</v>
       </c>
       <c r="K13" s="22"/>
-      <c r="L13" s="110" t="str">
+      <c r="L13" s="105" t="str">
         <f>IF(N13=0, "NOT STARTED",IF(N13&gt;D13, "ERROR TO MUCH WORK", IF(N13=D13, "DONE", "NOT ENOUGH WORK YET")))</f>
         <v>DONE</v>
       </c>
-      <c r="M13" s="111"/>
+      <c r="M13" s="106"/>
       <c r="N13" s="44">
         <f>SUM(E13:K13)</f>
         <v>1</v>
@@ -13089,10 +13175,10 @@
       <c r="P13" s="44"/>
     </row>
     <row r="14" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="106"/>
+      <c r="C14" s="101"/>
       <c r="D14" s="26">
         <v>0</v>
       </c>
@@ -13126,10 +13212,10 @@
       </c>
     </row>
     <row r="15" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="93"/>
+      <c r="C15" s="88"/>
       <c r="D15" s="32">
         <f>SUM(D6:D14)</f>
         <v>15.6</v>
@@ -13164,10 +13250,10 @@
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="95"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="39">
         <v>15.6</v>
       </c>
@@ -14212,12 +14298,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A8F48E-9C64-4E70-BB5A-3E5673E0A3CB}">
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14237,120 +14323,122 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="59"/>
-      <c r="E3" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
+      <c r="E3" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="88">
+      <c r="E4" s="76">
         <v>45978</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="79">
         <v>45979</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="79">
         <v>45980</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="79">
         <v>45981</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="79">
         <v>45982</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="79">
         <v>45983</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="79">
         <v>45984</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="102"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="91" t="s">
+      <c r="B5" s="97"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="81" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="72" t="s">
         <v>87</v>
       </c>
       <c r="C6" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="84">
         <v>1.5</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="108" t="str">
+      <c r="E6" s="77"/>
+      <c r="F6" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="103" t="str">
         <f t="shared" ref="L6:L23" si="0">IF(N6=0, "NOT STARTED",IF(N6&gt;D6, "ERROR TO MUCH WORK", IF(N6=D6, "DONE", "NOT ENOUGH WORK YET")))</f>
-        <v>NOT STARTED</v>
-      </c>
-      <c r="M6" s="109"/>
+        <v>NOT ENOUGH WORK YET</v>
+      </c>
+      <c r="M6" s="104"/>
       <c r="N6" s="44">
         <f t="shared" ref="N6:N23" si="1">SUM(E6:K6)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>47</v>
@@ -14358,60 +14446,64 @@
       <c r="P6" s="44"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="73" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="81">
+      <c r="D7" s="85">
         <v>1.5</v>
       </c>
-      <c r="E7" s="84"/>
+      <c r="E7" s="49">
+        <v>0.5</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
-      <c r="L7" s="108" t="str">
+      <c r="L7" s="103" t="str">
         <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-      <c r="M7" s="109"/>
+        <v>NOT ENOUGH WORK YET</v>
+      </c>
+      <c r="M7" s="104"/>
       <c r="N7" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>SUM(E7:K7)</f>
+        <v>0.5</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P7" s="44"/>
     </row>
-    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="86" t="s">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="73" t="s">
         <v>89</v>
       </c>
       <c r="C8" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="85">
         <v>1.5</v>
       </c>
-      <c r="E8" s="78">
-        <v>1</v>
-      </c>
-      <c r="F8" s="22"/>
+      <c r="E8" s="70">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.5</v>
+      </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="23"/>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
-      <c r="L8" s="108" t="str">
+      <c r="L8" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M8" s="109"/>
+      <c r="M8" s="104"/>
       <c r="N8" s="44">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -14422,30 +14514,34 @@
       <c r="P8" s="44"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="73" t="s">
         <v>90</v>
       </c>
       <c r="C9" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="85">
         <v>1.5</v>
       </c>
-      <c r="E9" s="78"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="70">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.5</v>
+      </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="23"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
-      <c r="L9" s="108" t="str">
+      <c r="L9" s="103" t="str">
         <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-      <c r="M9" s="109"/>
+        <v>NOT ENOUGH WORK YET</v>
+      </c>
+      <c r="M9" s="104"/>
       <c r="N9" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>99</v>
@@ -14453,27 +14549,27 @@
       <c r="P9" s="44"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="73" t="s">
         <v>91</v>
       </c>
       <c r="C10" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="81">
+      <c r="D10" s="85">
         <v>0.5</v>
       </c>
-      <c r="E10" s="78"/>
+      <c r="E10" s="70"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="23"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
-      <c r="L10" s="108" t="str">
+      <c r="L10" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M10" s="109"/>
+      <c r="M10" s="104"/>
       <c r="N10" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14483,17 +14579,17 @@
       </c>
       <c r="P10" s="44"/>
     </row>
-    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="86" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="73" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="82">
+      <c r="D11" s="85">
         <v>0.5</v>
       </c>
-      <c r="E11" s="78">
+      <c r="E11" s="70">
         <v>0.25</v>
       </c>
       <c r="F11" s="22"/>
@@ -14502,11 +14598,11 @@
       <c r="I11" s="23"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
-      <c r="L11" s="108" t="str">
+      <c r="L11" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M11" s="109"/>
+      <c r="M11" s="104"/>
       <c r="N11" s="44">
         <f t="shared" si="1"/>
         <v>0.25</v>
@@ -14517,27 +14613,27 @@
       <c r="P11" s="44"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="73" t="s">
         <v>93</v>
       </c>
       <c r="C12" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="80">
+      <c r="D12" s="85">
         <v>0.5</v>
       </c>
-      <c r="E12" s="78"/>
+      <c r="E12" s="70"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="23"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
-      <c r="L12" s="108" t="str">
+      <c r="L12" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M12" s="109"/>
+      <c r="M12" s="104"/>
       <c r="N12" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14548,27 +14644,27 @@
       <c r="P12" s="44"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="73" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="81">
+      <c r="D13" s="85">
         <v>0.5</v>
       </c>
-      <c r="E13" s="78"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
-      <c r="L13" s="108" t="str">
+      <c r="L13" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M13" s="109"/>
+      <c r="M13" s="104"/>
       <c r="N13" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14578,17 +14674,17 @@
       </c>
       <c r="P13" s="44"/>
     </row>
-    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="86">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="73">
         <v>35</v>
       </c>
       <c r="C14" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="82">
+      <c r="D14" s="85">
         <v>3</v>
       </c>
-      <c r="E14" s="78">
+      <c r="E14" s="70">
         <v>0.75</v>
       </c>
       <c r="F14" s="22"/>
@@ -14597,11 +14693,11 @@
       <c r="I14" s="23"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
-      <c r="L14" s="108" t="str">
+      <c r="L14" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT ENOUGH WORK YET</v>
       </c>
-      <c r="M14" s="109"/>
+      <c r="M14" s="104"/>
       <c r="N14" s="44">
         <f t="shared" si="1"/>
         <v>0.75</v>
@@ -14612,27 +14708,27 @@
       <c r="P14" s="44"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="86">
+      <c r="B15" s="73">
         <v>36</v>
       </c>
       <c r="C15" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="85">
         <v>3</v>
       </c>
-      <c r="E15" s="78"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
-      <c r="L15" s="108" t="str">
+      <c r="L15" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M15" s="109"/>
+      <c r="M15" s="104"/>
       <c r="N15" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14643,27 +14739,27 @@
       <c r="P15" s="44"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="73" t="s">
         <v>95</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="81">
+      <c r="D16" s="85">
         <v>1.5</v>
       </c>
-      <c r="E16" s="78"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="23"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
-      <c r="L16" s="108" t="str">
+      <c r="L16" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M16" s="109"/>
+      <c r="M16" s="104"/>
       <c r="N16" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14673,28 +14769,28 @@
       </c>
       <c r="P16" s="44"/>
     </row>
-    <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="86" t="s">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="73" t="s">
         <v>96</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="82">
+      <c r="D17" s="85">
         <v>1.5</v>
       </c>
-      <c r="E17" s="78"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="23"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
-      <c r="L17" s="108" t="str">
+      <c r="L17" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M17" s="109"/>
+      <c r="M17" s="104"/>
       <c r="N17" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14705,27 +14801,27 @@
       <c r="P17" s="44"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="73" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="85">
         <v>1.5</v>
       </c>
-      <c r="E18" s="78"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
       <c r="I18" s="23"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
-      <c r="L18" s="108" t="str">
+      <c r="L18" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M18" s="109"/>
+      <c r="M18" s="104"/>
       <c r="N18" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14736,27 +14832,27 @@
       <c r="P18" s="44"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="73" t="s">
         <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="81">
+      <c r="D19" s="85">
         <v>1.5</v>
       </c>
-      <c r="E19" s="78"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="23"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
-      <c r="L19" s="108" t="str">
+      <c r="L19" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M19" s="109"/>
+      <c r="M19" s="104"/>
       <c r="N19" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14766,28 +14862,28 @@
       </c>
       <c r="P19" s="44"/>
     </row>
-    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="86">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="73">
         <v>39</v>
       </c>
       <c r="C20" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="85">
         <v>3.5</v>
       </c>
-      <c r="E20" s="78"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="23"/>
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
-      <c r="L20" s="108" t="str">
+      <c r="L20" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M20" s="109"/>
+      <c r="M20" s="104"/>
       <c r="N20" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14798,27 +14894,27 @@
       <c r="P20" s="44"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="86">
+      <c r="B21" s="73">
         <v>40</v>
       </c>
       <c r="C21" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="80">
+      <c r="D21" s="85">
         <v>3.5</v>
       </c>
-      <c r="E21" s="78"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
-      <c r="L21" s="108" t="str">
+      <c r="L21" s="103" t="str">
         <f t="shared" si="0"/>
         <v>NOT STARTED</v>
       </c>
-      <c r="M21" s="109"/>
+      <c r="M21" s="104"/>
       <c r="N21" s="44">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -14829,30 +14925,34 @@
       <c r="P21" s="44"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="86">
+      <c r="B22" s="73">
         <v>41</v>
       </c>
       <c r="C22" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="81">
+      <c r="D22" s="85">
+        <v>2</v>
+      </c>
+      <c r="E22" s="70">
         <v>1</v>
       </c>
-      <c r="E22" s="78"/>
-      <c r="F22" s="22"/>
+      <c r="F22" s="22">
+        <v>1</v>
+      </c>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
       <c r="I22" s="23"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
-      <c r="L22" s="108" t="str">
+      <c r="L22" s="103" t="str">
         <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-      <c r="M22" s="109"/>
+        <v>DONE</v>
+      </c>
+      <c r="M22" s="104"/>
       <c r="N22" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>44</v>
@@ -14860,30 +14960,34 @@
       <c r="P22" s="44"/>
     </row>
     <row r="23" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="87">
+      <c r="B23" s="74">
         <v>42</v>
       </c>
-      <c r="C23" s="69" t="s">
+      <c r="C23" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="82">
-        <v>1</v>
-      </c>
-      <c r="E23" s="79"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="70"/>
-      <c r="L23" s="108" t="str">
+      <c r="D23" s="86">
+        <v>2</v>
+      </c>
+      <c r="E23" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="67">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="103" t="str">
         <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-      <c r="M23" s="109"/>
+        <v>NOT ENOUGH WORK YET</v>
+      </c>
+      <c r="M23" s="104"/>
       <c r="N23" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>39</v>
@@ -14891,129 +14995,129 @@
       <c r="P23" s="44"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="113"/>
-      <c r="D24" s="72">
+      <c r="C24" s="108"/>
+      <c r="D24" s="83">
         <v>0</v>
       </c>
-      <c r="E24" s="73">
-        <f t="shared" ref="E24:K24" ca="1" si="2">SUM(E6:E32)</f>
+      <c r="E24" s="69">
+        <f>SUM(E7:E23)</f>
+        <v>4</v>
+      </c>
+      <c r="F24" s="69">
+        <f t="shared" ref="F24:K24" si="2">SUM(F7:F23)</f>
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="69">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24" s="74">
-        <f t="shared" ca="1" si="2"/>
+      <c r="H24" s="69">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G24" s="74">
-        <f t="shared" ca="1" si="2"/>
+      <c r="I24" s="69">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H24" s="74">
-        <f t="shared" ca="1" si="2"/>
+      <c r="J24" s="69">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I24" s="75">
-        <f t="shared" ca="1" si="2"/>
+      <c r="K24" s="69">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="76">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="77">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="108"/>
-      <c r="M24" s="109"/>
+      <c r="L24" s="103"/>
+      <c r="M24" s="104"/>
       <c r="N24" s="44"/>
       <c r="O24" s="44"/>
       <c r="P24" s="44"/>
     </row>
     <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="114" t="s">
+      <c r="B25" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="113"/>
+      <c r="C25" s="108"/>
       <c r="D25" s="64">
         <f>SUM(D6:D24)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E25" s="65">
-        <f t="shared" ref="E25:K25" ca="1" si="3">D25-SUM(E6:E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="67">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="68">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="108"/>
-      <c r="M25" s="109"/>
+        <f>D25-SUM(E7:E23)</f>
+        <v>27</v>
+      </c>
+      <c r="F25" s="65">
+        <f t="shared" ref="F25:K25" si="3">E25-SUM(F7:F23)</f>
+        <v>24.5</v>
+      </c>
+      <c r="G25" s="65">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="H25" s="65">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="I25" s="65">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="J25" s="65">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="K25" s="65">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="L25" s="103"/>
+      <c r="M25" s="104"/>
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
       <c r="P25" s="44"/>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="115" t="s">
+      <c r="B26" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="116"/>
+      <c r="C26" s="111"/>
       <c r="D26" s="61">
         <f>SUM(D6:D23)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E26" s="62">
         <f>$D$26-($D$26/7*1)</f>
-        <v>24.857142857142858</v>
+        <v>26.571428571428569</v>
       </c>
       <c r="F26" s="62">
         <f>$D$26-($D$26/7*2)</f>
-        <v>20.714285714285715</v>
+        <v>22.142857142857142</v>
       </c>
       <c r="G26" s="62">
         <f>$D$26-($D$26/7*3)</f>
-        <v>16.571428571428569</v>
+        <v>17.714285714285715</v>
       </c>
       <c r="H26" s="62">
         <f>$D$26-($D$26/7*4)</f>
-        <v>12.428571428571427</v>
+        <v>13.285714285714285</v>
       </c>
       <c r="I26" s="62">
         <f>$D$26-($D$26/7*5)</f>
-        <v>8.2857142857142847</v>
+        <v>8.8571428571428541</v>
       </c>
       <c r="J26" s="62">
         <f>$D$26-($D$26/7*6)</f>
-        <v>4.1428571428571388</v>
+        <v>4.428571428571427</v>
       </c>
       <c r="K26" s="63">
         <f>$D$26-($D$26/7*7)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="108"/>
-      <c r="M26" s="109"/>
+      <c r="L26" s="103"/>
+      <c r="M26" s="104"/>
       <c r="N26" s="44"/>
       <c r="O26" s="44"/>
       <c r="P26" s="44"/>
@@ -15029,8 +15133,8 @@
       <c r="I27" s="59"/>
       <c r="J27" s="59"/>
       <c r="K27" s="59"/>
-      <c r="L27" s="108"/>
-      <c r="M27" s="109"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="104"/>
       <c r="N27" s="44"/>
       <c r="O27" s="44"/>
       <c r="P27" s="44"/>
@@ -15046,8 +15150,8 @@
       <c r="I28" s="59"/>
       <c r="J28" s="59"/>
       <c r="K28" s="59"/>
-      <c r="L28" s="108"/>
-      <c r="M28" s="109"/>
+      <c r="L28" s="103"/>
+      <c r="M28" s="104"/>
       <c r="N28" s="44"/>
       <c r="O28" s="44"/>
       <c r="P28" s="44"/>
@@ -15063,8 +15167,8 @@
       <c r="I29" s="59"/>
       <c r="J29" s="59"/>
       <c r="K29" s="59"/>
-      <c r="L29" s="108"/>
-      <c r="M29" s="109"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="104"/>
       <c r="N29" s="44"/>
       <c r="O29" s="44"/>
       <c r="P29" s="44"/>
@@ -15080,8 +15184,8 @@
       <c r="I30" s="59"/>
       <c r="J30" s="59"/>
       <c r="K30" s="59"/>
-      <c r="L30" s="108"/>
-      <c r="M30" s="109"/>
+      <c r="L30" s="103"/>
+      <c r="M30" s="104"/>
       <c r="N30" s="44"/>
       <c r="O30" s="44"/>
       <c r="P30" s="44"/>
@@ -15097,8 +15201,8 @@
       <c r="I31" s="59"/>
       <c r="J31" s="59"/>
       <c r="K31" s="59"/>
-      <c r="L31" s="108"/>
-      <c r="M31" s="109"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="104"/>
       <c r="N31" s="44"/>
       <c r="O31" s="44"/>
       <c r="P31" s="44"/>
@@ -15114,8 +15218,8 @@
       <c r="I32" s="59"/>
       <c r="J32" s="59"/>
       <c r="K32" s="59"/>
-      <c r="L32" s="108"/>
-      <c r="M32" s="109"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="104"/>
       <c r="N32" s="44"/>
       <c r="O32" s="44"/>
       <c r="P32" s="44"/>
@@ -15131,8 +15235,8 @@
       <c r="I33" s="59"/>
       <c r="J33" s="59"/>
       <c r="K33" s="59"/>
-      <c r="L33" s="108"/>
-      <c r="M33" s="109"/>
+      <c r="L33" s="103"/>
+      <c r="M33" s="104"/>
       <c r="N33" s="44"/>
       <c r="O33" s="44"/>
       <c r="P33" s="44"/>
@@ -15148,8 +15252,8 @@
       <c r="I34" s="59"/>
       <c r="J34" s="59"/>
       <c r="K34" s="59"/>
-      <c r="L34" s="108"/>
-      <c r="M34" s="109"/>
+      <c r="L34" s="103"/>
+      <c r="M34" s="104"/>
       <c r="N34" s="44"/>
       <c r="O34" s="44"/>
       <c r="P34" s="44"/>
@@ -15165,8 +15269,8 @@
       <c r="I35" s="59"/>
       <c r="J35" s="59"/>
       <c r="K35" s="59"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="109"/>
+      <c r="L35" s="103"/>
+      <c r="M35" s="104"/>
       <c r="N35" s="44"/>
       <c r="O35" s="44"/>
       <c r="P35" s="44"/>
@@ -15182,8 +15286,8 @@
       <c r="I36" s="59"/>
       <c r="J36" s="59"/>
       <c r="K36" s="59"/>
-      <c r="L36" s="108"/>
-      <c r="M36" s="109"/>
+      <c r="L36" s="103"/>
+      <c r="M36" s="104"/>
       <c r="N36" s="44"/>
       <c r="O36" s="44"/>
       <c r="P36" s="44"/>
@@ -15199,8 +15303,8 @@
       <c r="I37" s="59"/>
       <c r="J37" s="59"/>
       <c r="K37" s="59"/>
-      <c r="L37" s="108"/>
-      <c r="M37" s="109"/>
+      <c r="L37" s="103"/>
+      <c r="M37" s="104"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
       <c r="P37" s="44"/>
@@ -15263,7 +15367,7 @@
       <formula>"NOT STARTED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N37">
+  <conditionalFormatting sqref="N6:N37">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>

</xml_diff>